<commit_message>
s8812_earned_income_worksheet.xlsx - bold one word
</commit_message>
<xml_diff>
--- a/Federal/s8812_earned_income_worksheet.xlsx
+++ b/Federal/s8812_earned_income_worksheet.xlsx
@@ -72,9 +72,6 @@
     <t>3</t>
   </si>
   <si>
-    <t>Combine lines 1a, 1b, 2a, 2b, and 2e. If zero or less, stop. Do not complete the rest of this worksheet. Instead, enter -0- on line 3 of Credit Limit Worksheet B or line 18a of Schedule 8812, whichever applies</t>
-  </si>
-  <si>
     <t>4</t>
   </si>
   <si>
@@ -208,6 +205,30 @@
   </si>
   <si>
     <t>Earned Income Worksheet</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Combine lines 1a, 1b, 2a, 2b, and 2e. If zero or less, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>stop</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="2"/>
+      </rPr>
+      <t>. Do not complete the rest of this worksheet. Instead, enter -0- on line 3 of Credit Limit Worksheet B or line 18a of Schedule 8812, whichever applies</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -903,10 +924,6 @@
   <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top"/>
     </xf>
@@ -917,13 +934,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
@@ -931,16 +942,7 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="20" fillId="33" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="20" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="20" fillId="33" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="21" xfId="0" applyFill="1" applyBorder="1"/>
@@ -959,6 +961,53 @@
     <xf numFmtId="44" fontId="0" fillId="0" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="20" fillId="33" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="33" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -968,34 +1017,6 @@
     <xf numFmtId="0" fontId="0" fillId="33" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="20" builtinId="30" customBuiltin="1"/>
@@ -1325,8 +1346,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N31" sqref="N31"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="202" zoomScaleNormal="202" workbookViewId="0">
+      <selection activeCell="B41" sqref="B41:F41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1340,284 +1361,284 @@
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="45" t="s">
+      <c r="B1" s="30" t="s">
+        <v>61</v>
+      </c>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
+      <c r="G1" s="30"/>
+      <c r="H1" s="30"/>
+      <c r="I1" s="30"/>
+      <c r="J1" s="30"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="36" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="36"/>
+      <c r="D2" s="36"/>
+      <c r="E2" s="36"/>
+      <c r="F2" s="36"/>
+      <c r="G2" s="36"/>
+      <c r="H2" s="36"/>
+      <c r="I2" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="J2" s="20"/>
+    </row>
+    <row r="3" spans="1:10" ht="66" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="31" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="31"/>
+      <c r="D3" s="31"/>
+      <c r="E3" s="31"/>
+      <c r="F3" s="31"/>
+      <c r="G3" s="31"/>
+      <c r="H3" s="31"/>
+      <c r="I3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="J3" s="22"/>
+    </row>
+    <row r="4" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="44" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="45"/>
+      <c r="C4" s="45"/>
+      <c r="D4" s="45"/>
+      <c r="E4" s="45"/>
+      <c r="F4" s="45"/>
+      <c r="G4" s="45"/>
+      <c r="H4" s="45"/>
+      <c r="I4" s="45"/>
+      <c r="J4" s="46"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="31" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="31"/>
+      <c r="D5" s="31"/>
+      <c r="E5" s="31"/>
+      <c r="F5" s="31"/>
+      <c r="G5" s="31"/>
+      <c r="H5" s="31"/>
+      <c r="I5" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="J5" s="22"/>
+    </row>
+    <row r="6" spans="1:10" ht="126" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="21" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="31" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="31"/>
+      <c r="D6" s="31"/>
+      <c r="E6" s="31"/>
+      <c r="F6" s="31"/>
+      <c r="G6" s="31"/>
+      <c r="H6" s="31"/>
+      <c r="I6" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="J6" s="22"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="31" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="31"/>
+      <c r="D7" s="31"/>
+      <c r="E7" s="31"/>
+      <c r="F7" s="31"/>
+      <c r="G7" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="H7" s="4"/>
+      <c r="I7" s="23"/>
+      <c r="J7" s="24"/>
+    </row>
+    <row r="8" spans="1:10" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" s="31" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" s="31"/>
+      <c r="D8" s="31"/>
+      <c r="E8" s="31"/>
+      <c r="F8" s="31"/>
+      <c r="G8" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H8" s="4"/>
+      <c r="I8" s="23"/>
+      <c r="J8" s="24"/>
+    </row>
+    <row r="9" spans="1:10" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" s="31" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" s="31"/>
+      <c r="D9" s="31"/>
+      <c r="E9" s="31"/>
+      <c r="F9" s="31"/>
+      <c r="G9" s="31"/>
+      <c r="H9" s="31"/>
+      <c r="I9" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="J9" s="22"/>
+    </row>
+    <row r="10" spans="1:10" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" s="31" t="s">
         <v>62</v>
       </c>
-      <c r="C1" s="45"/>
-      <c r="D1" s="45"/>
-      <c r="E1" s="45"/>
-      <c r="F1" s="45"/>
-      <c r="G1" s="45"/>
-      <c r="H1" s="45"/>
-      <c r="I1" s="45"/>
-      <c r="J1" s="45"/>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="29" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
-      <c r="F2" s="10"/>
-      <c r="G2" s="10"/>
-      <c r="H2" s="10"/>
-      <c r="I2" s="30" t="s">
-        <v>1</v>
-      </c>
-      <c r="J2" s="31"/>
-    </row>
-    <row r="3" spans="1:10" ht="66" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="32" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-      <c r="I3" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="J3" s="33"/>
-    </row>
-    <row r="4" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="34" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" s="35"/>
-      <c r="C4" s="35"/>
-      <c r="D4" s="35"/>
-      <c r="E4" s="35"/>
-      <c r="F4" s="35"/>
-      <c r="G4" s="35"/>
-      <c r="H4" s="35"/>
-      <c r="I4" s="35"/>
-      <c r="J4" s="36"/>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="32" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2"/>
-      <c r="I5" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="J5" s="33"/>
-    </row>
-    <row r="6" spans="1:10" ht="126" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="32" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
-      <c r="I6" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="J6" s="33"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="32" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="H7" s="6"/>
-      <c r="I7" s="37"/>
-      <c r="J7" s="38"/>
-    </row>
-    <row r="8" spans="1:10" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="32" t="s">
-        <v>12</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="H8" s="6"/>
-      <c r="I8" s="37"/>
-      <c r="J8" s="38"/>
-    </row>
-    <row r="9" spans="1:10" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="32" t="s">
-        <v>14</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
-      <c r="H9" s="2"/>
-      <c r="I9" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="J9" s="33"/>
-    </row>
-    <row r="10" spans="1:10" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="32" t="s">
+      <c r="C10" s="31"/>
+      <c r="D10" s="31"/>
+      <c r="E10" s="31"/>
+      <c r="F10" s="31"/>
+      <c r="G10" s="31"/>
+      <c r="H10" s="31"/>
+      <c r="I10" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
-      <c r="H10" s="2"/>
-      <c r="I10" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="J10" s="33">
+      <c r="J10" s="22">
         <f>SUM(J2:J9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="32" t="s">
+      <c r="A11" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" s="31" t="s">
         <v>18</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="C11" s="31"/>
+      <c r="D11" s="31"/>
+      <c r="E11" s="31"/>
+      <c r="F11" s="31"/>
+      <c r="G11" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H11" s="4"/>
+      <c r="I11" s="23"/>
+      <c r="J11" s="24"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-      <c r="G11" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="H11" s="6"/>
-      <c r="I11" s="37"/>
-      <c r="J11" s="38"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="32" t="s">
+      <c r="B12" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="C12" s="31"/>
+      <c r="D12" s="31"/>
+      <c r="E12" s="31"/>
+      <c r="F12" s="31"/>
+      <c r="G12" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="H12" s="4"/>
+      <c r="I12" s="23"/>
+      <c r="J12" s="24"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
-      <c r="G12" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="H12" s="6"/>
-      <c r="I12" s="37"/>
-      <c r="J12" s="38"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="32" t="s">
+      <c r="B13" s="31" t="s">
         <v>22</v>
       </c>
-      <c r="B13" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
-      <c r="G13" s="2"/>
-      <c r="H13" s="2"/>
-      <c r="I13" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="J13" s="33">
+      <c r="C13" s="31"/>
+      <c r="D13" s="31"/>
+      <c r="E13" s="31"/>
+      <c r="F13" s="31"/>
+      <c r="G13" s="31"/>
+      <c r="H13" s="31"/>
+      <c r="I13" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="J13" s="22">
         <f>H11+H12</f>
         <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="32" t="s">
+      <c r="A14" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="B14" s="31" t="s">
         <v>24</v>
       </c>
-      <c r="B14" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
-      <c r="G14" s="2"/>
-      <c r="H14" s="2"/>
-      <c r="I14" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="J14" s="33">
+      <c r="C14" s="31"/>
+      <c r="D14" s="31"/>
+      <c r="E14" s="31"/>
+      <c r="F14" s="31"/>
+      <c r="G14" s="31"/>
+      <c r="H14" s="31"/>
+      <c r="I14" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="J14" s="22">
         <f>J10-J13</f>
         <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="39" t="s">
+      <c r="A15" s="37" t="s">
+        <v>25</v>
+      </c>
+      <c r="B15" s="38"/>
+      <c r="C15" s="38"/>
+      <c r="D15" s="38"/>
+      <c r="E15" s="38"/>
+      <c r="F15" s="38"/>
+      <c r="G15" s="38"/>
+      <c r="H15" s="38"/>
+      <c r="I15" s="38"/>
+      <c r="J15" s="39"/>
+    </row>
+    <row r="16" spans="1:10" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="40" t="s">
         <v>26</v>
       </c>
-      <c r="B15" s="40"/>
-      <c r="C15" s="40"/>
-      <c r="D15" s="40"/>
-      <c r="E15" s="40"/>
-      <c r="F15" s="40"/>
-      <c r="G15" s="40"/>
-      <c r="H15" s="40"/>
-      <c r="I15" s="40"/>
-      <c r="J15" s="41"/>
-    </row>
-    <row r="16" spans="1:10" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="42" t="s">
-        <v>27</v>
-      </c>
-      <c r="B16" s="43"/>
-      <c r="C16" s="43"/>
-      <c r="D16" s="43"/>
-      <c r="E16" s="43"/>
-      <c r="F16" s="43"/>
-      <c r="G16" s="43"/>
-      <c r="H16" s="43"/>
-      <c r="I16" s="43"/>
-      <c r="J16" s="44"/>
+      <c r="B16" s="41"/>
+      <c r="C16" s="41"/>
+      <c r="D16" s="41"/>
+      <c r="E16" s="41"/>
+      <c r="F16" s="41"/>
+      <c r="G16" s="41"/>
+      <c r="H16" s="41"/>
+      <c r="I16" s="41"/>
+      <c r="J16" s="42"/>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
@@ -1625,18 +1646,18 @@
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A18" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="B18" s="3"/>
-      <c r="C18" s="3"/>
-      <c r="D18" s="3"/>
-      <c r="E18" s="3"/>
-      <c r="F18" s="3"/>
-      <c r="G18" s="3"/>
-      <c r="H18" s="3"/>
-      <c r="I18" s="3"/>
-      <c r="J18" s="3"/>
+      <c r="A18" s="35" t="s">
+        <v>27</v>
+      </c>
+      <c r="B18" s="35"/>
+      <c r="C18" s="35"/>
+      <c r="D18" s="35"/>
+      <c r="E18" s="35"/>
+      <c r="F18" s="35"/>
+      <c r="G18" s="35"/>
+      <c r="H18" s="35"/>
+      <c r="I18" s="35"/>
+      <c r="J18" s="35"/>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
@@ -1644,394 +1665,417 @@
       </c>
     </row>
     <row r="20" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A20" s="8" t="s">
+      <c r="A20" s="43" t="s">
+        <v>28</v>
+      </c>
+      <c r="B20" s="43"/>
+      <c r="C20" s="43"/>
+      <c r="D20" s="43"/>
+      <c r="E20" s="43"/>
+      <c r="F20" s="43"/>
+      <c r="G20" s="43"/>
+      <c r="H20" s="43"/>
+      <c r="I20" s="43"/>
+      <c r="J20" s="43"/>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21" s="35" t="s">
         <v>29</v>
       </c>
-      <c r="B20" s="8"/>
-      <c r="C20" s="8"/>
-      <c r="D20" s="8"/>
-      <c r="E20" s="8"/>
-      <c r="F20" s="8"/>
-      <c r="G20" s="8"/>
-      <c r="H20" s="8"/>
-      <c r="I20" s="8"/>
-      <c r="J20" s="8"/>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A21" s="3" t="s">
+      <c r="B21" s="35"/>
+      <c r="C21" s="35"/>
+      <c r="D21" s="35"/>
+      <c r="E21" s="35"/>
+      <c r="F21" s="35"/>
+      <c r="G21" s="35"/>
+      <c r="H21" s="35"/>
+      <c r="I21" s="35"/>
+      <c r="J21" s="35"/>
+    </row>
+    <row r="22" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="35" t="s">
         <v>30</v>
       </c>
-      <c r="B21" s="3"/>
-      <c r="C21" s="3"/>
-      <c r="D21" s="3"/>
-      <c r="E21" s="3"/>
-      <c r="F21" s="3"/>
-      <c r="G21" s="3"/>
-      <c r="H21" s="3"/>
-      <c r="I21" s="3"/>
-      <c r="J21" s="3"/>
-    </row>
-    <row r="22" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="3" t="s">
+      <c r="B22" s="35"/>
+      <c r="C22" s="35"/>
+      <c r="D22" s="35"/>
+      <c r="E22" s="35"/>
+      <c r="F22" s="35"/>
+      <c r="G22" s="35"/>
+      <c r="H22" s="35"/>
+      <c r="I22" s="35"/>
+      <c r="J22" s="35"/>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A23" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="B22" s="3"/>
-      <c r="C22" s="3"/>
-      <c r="D22" s="3"/>
-      <c r="E22" s="3"/>
-      <c r="F22" s="3"/>
-      <c r="G22" s="3"/>
-      <c r="H22" s="3"/>
-      <c r="I22" s="3"/>
-      <c r="J22" s="3"/>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A23" s="9" t="s">
+      <c r="B23" s="36" t="s">
         <v>32</v>
       </c>
-      <c r="B23" s="10" t="s">
+      <c r="C23" s="36"/>
+      <c r="D23" s="36"/>
+      <c r="E23" s="36"/>
+      <c r="F23" s="36"/>
+      <c r="G23" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="H23" s="8"/>
+      <c r="I23" s="9"/>
+      <c r="J23" s="10"/>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A24" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="C23" s="10"/>
-      <c r="D23" s="10"/>
-      <c r="E23" s="10"/>
-      <c r="F23" s="10"/>
-      <c r="G23" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="H23" s="12"/>
-      <c r="I23" s="13"/>
-      <c r="J23" s="14"/>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A24" s="15" t="s">
+      <c r="B24" s="31" t="s">
         <v>34</v>
       </c>
-      <c r="B24" s="2" t="s">
+      <c r="C24" s="31"/>
+      <c r="D24" s="31"/>
+      <c r="E24" s="31"/>
+      <c r="F24" s="31"/>
+      <c r="G24" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H24" s="5"/>
+      <c r="I24" s="12"/>
+      <c r="J24" s="13"/>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A25" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="B25" s="31" t="s">
         <v>35</v>
       </c>
-      <c r="C24" s="2"/>
-      <c r="D24" s="2"/>
-      <c r="E24" s="2"/>
-      <c r="F24" s="2"/>
-      <c r="G24" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="H24" s="7"/>
-      <c r="I24" s="16"/>
-      <c r="J24" s="17"/>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A25" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="C25" s="2"/>
-      <c r="D25" s="2"/>
-      <c r="E25" s="2"/>
-      <c r="F25" s="2"/>
+      <c r="C25" s="31"/>
+      <c r="D25" s="31"/>
+      <c r="E25" s="31"/>
+      <c r="F25" s="31"/>
       <c r="G25" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="H25" s="7"/>
-      <c r="I25" s="16"/>
-      <c r="J25" s="17"/>
+      <c r="H25" s="5"/>
+      <c r="I25" s="12"/>
+      <c r="J25" s="13"/>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A26" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="C26" s="2"/>
-      <c r="D26" s="2"/>
-      <c r="E26" s="2"/>
-      <c r="F26" s="2"/>
+      <c r="A26" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="B26" s="31" t="s">
+        <v>36</v>
+      </c>
+      <c r="C26" s="31"/>
+      <c r="D26" s="31"/>
+      <c r="E26" s="31"/>
+      <c r="F26" s="31"/>
       <c r="G26" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="H26" s="7">
+        <v>17</v>
+      </c>
+      <c r="H26" s="5">
         <f>SUM(H23:H25)</f>
         <v>0</v>
       </c>
-      <c r="I26" s="16"/>
-      <c r="J26" s="17"/>
+      <c r="I26" s="12"/>
+      <c r="J26" s="13"/>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A27" s="15" t="s">
-        <v>20</v>
-      </c>
-      <c r="B27" s="2" t="s">
+      <c r="A27" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="B27" s="31" t="s">
+        <v>37</v>
+      </c>
+      <c r="C27" s="31"/>
+      <c r="D27" s="31"/>
+      <c r="E27" s="31"/>
+      <c r="F27" s="31"/>
+      <c r="G27" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H27" s="5"/>
+      <c r="I27" s="12"/>
+      <c r="J27" s="13"/>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A28" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="B28" s="31" t="s">
         <v>38</v>
       </c>
-      <c r="C27" s="2"/>
-      <c r="D27" s="2"/>
-      <c r="E27" s="2"/>
-      <c r="F27" s="2"/>
-      <c r="G27" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="H27" s="7"/>
-      <c r="I27" s="16"/>
-      <c r="J27" s="17"/>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A28" s="15" t="s">
-        <v>22</v>
-      </c>
-      <c r="B28" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="C28" s="2"/>
-      <c r="D28" s="2"/>
-      <c r="E28" s="2"/>
-      <c r="F28" s="2"/>
+      <c r="C28" s="31"/>
+      <c r="D28" s="31"/>
+      <c r="E28" s="31"/>
+      <c r="F28" s="31"/>
       <c r="G28" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="H28" s="7">
+        <v>21</v>
+      </c>
+      <c r="H28" s="5">
         <f>H26-H27</f>
         <v>0</v>
       </c>
-      <c r="I28" s="16"/>
-      <c r="J28" s="17"/>
+      <c r="I28" s="12"/>
+      <c r="J28" s="13"/>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A29" s="18" t="s">
+      <c r="A29" s="32" t="s">
+        <v>39</v>
+      </c>
+      <c r="B29" s="33"/>
+      <c r="C29" s="33"/>
+      <c r="D29" s="33"/>
+      <c r="E29" s="33"/>
+      <c r="F29" s="33"/>
+      <c r="G29" s="33"/>
+      <c r="H29" s="33"/>
+      <c r="I29" s="33"/>
+      <c r="J29" s="34"/>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A30" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="B30" s="31" t="s">
         <v>40</v>
       </c>
-      <c r="B29" s="19"/>
-      <c r="C29" s="19"/>
-      <c r="D29" s="19"/>
-      <c r="E29" s="19"/>
-      <c r="F29" s="19"/>
-      <c r="G29" s="19"/>
-      <c r="H29" s="19"/>
-      <c r="I29" s="19"/>
-      <c r="J29" s="20"/>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A30" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="B30" s="2" t="s">
+      <c r="C30" s="31"/>
+      <c r="D30" s="31"/>
+      <c r="E30" s="31"/>
+      <c r="F30" s="31"/>
+      <c r="G30" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H30" s="5"/>
+      <c r="I30" s="12"/>
+      <c r="J30" s="13"/>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A31" s="32" t="s">
         <v>41</v>
       </c>
-      <c r="C30" s="2"/>
-      <c r="D30" s="2"/>
-      <c r="E30" s="2"/>
-      <c r="F30" s="2"/>
-      <c r="G30" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="H30" s="7"/>
-      <c r="I30" s="16"/>
-      <c r="J30" s="17"/>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A31" s="18" t="s">
+      <c r="B31" s="33"/>
+      <c r="C31" s="33"/>
+      <c r="D31" s="33"/>
+      <c r="E31" s="33"/>
+      <c r="F31" s="33"/>
+      <c r="G31" s="33"/>
+      <c r="H31" s="33"/>
+      <c r="I31" s="33"/>
+      <c r="J31" s="34"/>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A32" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="B31" s="19"/>
-      <c r="C31" s="19"/>
-      <c r="D31" s="19"/>
-      <c r="E31" s="19"/>
-      <c r="F31" s="19"/>
-      <c r="G31" s="19"/>
-      <c r="H31" s="19"/>
-      <c r="I31" s="19"/>
-      <c r="J31" s="20"/>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A32" s="15" t="s">
+      <c r="B32" s="31" t="s">
         <v>43</v>
       </c>
-      <c r="B32" s="2" t="s">
+      <c r="C32" s="31"/>
+      <c r="D32" s="31"/>
+      <c r="E32" s="31"/>
+      <c r="F32" s="31"/>
+      <c r="G32" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="H32" s="5"/>
+      <c r="I32" s="12"/>
+      <c r="J32" s="13"/>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A33" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="C32" s="2"/>
-      <c r="D32" s="2"/>
-      <c r="E32" s="2"/>
-      <c r="F32" s="2"/>
-      <c r="G32" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="H32" s="7"/>
-      <c r="I32" s="16"/>
-      <c r="J32" s="17"/>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A33" s="15" t="s">
+      <c r="B33" s="31" t="s">
         <v>45</v>
       </c>
-      <c r="B33" s="2" t="s">
+      <c r="C33" s="31"/>
+      <c r="D33" s="31"/>
+      <c r="E33" s="31"/>
+      <c r="F33" s="31"/>
+      <c r="G33" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="H33" s="5"/>
+      <c r="I33" s="12"/>
+      <c r="J33" s="13"/>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A34" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="C33" s="2"/>
-      <c r="D33" s="2"/>
-      <c r="E33" s="2"/>
-      <c r="F33" s="2"/>
-      <c r="G33" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="H33" s="7"/>
-      <c r="I33" s="16"/>
-      <c r="J33" s="17"/>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A34" s="15" t="s">
+      <c r="B34" s="31" t="s">
         <v>47</v>
       </c>
-      <c r="B34" s="2" t="s">
+      <c r="C34" s="31"/>
+      <c r="D34" s="31"/>
+      <c r="E34" s="31"/>
+      <c r="F34" s="31"/>
+      <c r="G34" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="H34" s="5"/>
+      <c r="I34" s="12"/>
+      <c r="J34" s="13"/>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A35" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="C34" s="2"/>
-      <c r="D34" s="2"/>
-      <c r="E34" s="2"/>
-      <c r="F34" s="2"/>
-      <c r="G34" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="H34" s="7"/>
-      <c r="I34" s="16"/>
-      <c r="J34" s="17"/>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A35" s="15" t="s">
+      <c r="B35" s="31" t="s">
         <v>49</v>
       </c>
-      <c r="B35" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="C35" s="2"/>
-      <c r="D35" s="2"/>
-      <c r="E35" s="2"/>
-      <c r="F35" s="2"/>
+      <c r="C35" s="31"/>
+      <c r="D35" s="31"/>
+      <c r="E35" s="31"/>
+      <c r="F35" s="31"/>
       <c r="G35" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="H35" s="7">
+        <v>48</v>
+      </c>
+      <c r="H35" s="5">
         <f>SUM(H32:H34)</f>
         <v>0</v>
       </c>
-      <c r="I35" s="16"/>
-      <c r="J35" s="17"/>
+      <c r="I35" s="12"/>
+      <c r="J35" s="13"/>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A36" s="15" t="s">
+      <c r="A36" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="B36" s="31" t="s">
         <v>51</v>
       </c>
-      <c r="B36" s="2" t="s">
+      <c r="C36" s="31"/>
+      <c r="D36" s="31"/>
+      <c r="E36" s="31"/>
+      <c r="F36" s="31"/>
+      <c r="G36" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="H36" s="5"/>
+      <c r="I36" s="12"/>
+      <c r="J36" s="13"/>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A37" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="C36" s="2"/>
-      <c r="D36" s="2"/>
-      <c r="E36" s="2"/>
-      <c r="F36" s="2"/>
-      <c r="G36" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="H36" s="7"/>
-      <c r="I36" s="16"/>
-      <c r="J36" s="17"/>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A37" s="15" t="s">
+      <c r="B37" s="31" t="s">
         <v>53</v>
       </c>
-      <c r="B37" s="2" t="s">
+      <c r="C37" s="31"/>
+      <c r="D37" s="31"/>
+      <c r="E37" s="31"/>
+      <c r="F37" s="31"/>
+      <c r="G37" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="H37" s="5"/>
+      <c r="I37" s="12"/>
+      <c r="J37" s="13"/>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A38" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="C37" s="2"/>
-      <c r="D37" s="2"/>
-      <c r="E37" s="2"/>
-      <c r="F37" s="2"/>
-      <c r="G37" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="H37" s="7"/>
-      <c r="I37" s="16"/>
-      <c r="J37" s="17"/>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A38" s="15" t="s">
+      <c r="B38" s="31" t="s">
         <v>55</v>
       </c>
-      <c r="B38" s="2" t="s">
+      <c r="C38" s="31"/>
+      <c r="D38" s="31"/>
+      <c r="E38" s="31"/>
+      <c r="F38" s="31"/>
+      <c r="G38" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="H38" s="5"/>
+      <c r="I38" s="12"/>
+      <c r="J38" s="13"/>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A39" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="C38" s="2"/>
-      <c r="D38" s="2"/>
-      <c r="E38" s="2"/>
-      <c r="F38" s="2"/>
-      <c r="G38" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="H38" s="7"/>
-      <c r="I38" s="16"/>
-      <c r="J38" s="17"/>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A39" s="15" t="s">
+      <c r="B39" s="31" t="s">
         <v>57</v>
       </c>
-      <c r="B39" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="C39" s="2"/>
-      <c r="D39" s="2"/>
-      <c r="E39" s="2"/>
-      <c r="F39" s="2"/>
+      <c r="C39" s="31"/>
+      <c r="D39" s="31"/>
+      <c r="E39" s="31"/>
+      <c r="F39" s="31"/>
       <c r="G39" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="H39" s="7">
+        <v>56</v>
+      </c>
+      <c r="H39" s="5">
         <f>SUM(H36:H38)</f>
         <v>0</v>
       </c>
-      <c r="I39" s="16"/>
-      <c r="J39" s="17"/>
+      <c r="I39" s="12"/>
+      <c r="J39" s="13"/>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A40" s="21" t="s">
+      <c r="A40" s="26" t="s">
+        <v>58</v>
+      </c>
+      <c r="B40" s="27"/>
+      <c r="C40" s="27"/>
+      <c r="D40" s="27"/>
+      <c r="E40" s="27"/>
+      <c r="F40" s="27"/>
+      <c r="G40" s="27"/>
+      <c r="H40" s="27"/>
+      <c r="I40" s="27"/>
+      <c r="J40" s="28"/>
+    </row>
+    <row r="41" spans="1:10" ht="53.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="14" t="s">
         <v>59</v>
       </c>
-      <c r="B40" s="22"/>
-      <c r="C40" s="22"/>
-      <c r="D40" s="22"/>
-      <c r="E40" s="22"/>
-      <c r="F40" s="22"/>
-      <c r="G40" s="22"/>
-      <c r="H40" s="22"/>
-      <c r="I40" s="22"/>
-      <c r="J40" s="23"/>
-    </row>
-    <row r="41" spans="1:10" ht="53.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="24" t="s">
+      <c r="B41" s="29" t="s">
         <v>60</v>
       </c>
-      <c r="B41" s="25" t="s">
-        <v>61</v>
-      </c>
-      <c r="C41" s="25"/>
-      <c r="D41" s="25"/>
-      <c r="E41" s="25"/>
-      <c r="F41" s="25"/>
-      <c r="G41" s="26" t="s">
-        <v>60</v>
-      </c>
-      <c r="H41" s="46">
+      <c r="C41" s="29"/>
+      <c r="D41" s="29"/>
+      <c r="E41" s="29"/>
+      <c r="F41" s="29"/>
+      <c r="G41" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="H41" s="25">
         <f>H28+H30+H35+H39</f>
         <v>0</v>
       </c>
-      <c r="I41" s="27"/>
-      <c r="J41" s="28"/>
+      <c r="I41" s="16"/>
+      <c r="J41" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="39">
+    <mergeCell ref="B7:F7"/>
+    <mergeCell ref="B2:H2"/>
+    <mergeCell ref="B3:H3"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="B5:H5"/>
+    <mergeCell ref="B6:H6"/>
+    <mergeCell ref="A21:J21"/>
+    <mergeCell ref="B8:F8"/>
+    <mergeCell ref="B9:H9"/>
+    <mergeCell ref="B10:H10"/>
+    <mergeCell ref="B11:F11"/>
+    <mergeCell ref="B12:F12"/>
+    <mergeCell ref="B13:H13"/>
+    <mergeCell ref="B14:H14"/>
+    <mergeCell ref="A15:J15"/>
+    <mergeCell ref="A16:J16"/>
+    <mergeCell ref="A18:J18"/>
+    <mergeCell ref="A20:J20"/>
+    <mergeCell ref="B23:F23"/>
+    <mergeCell ref="B24:F24"/>
+    <mergeCell ref="B25:F25"/>
+    <mergeCell ref="B26:F26"/>
+    <mergeCell ref="B27:F27"/>
     <mergeCell ref="A40:J40"/>
     <mergeCell ref="B41:F41"/>
     <mergeCell ref="B1:J1"/>
@@ -2048,29 +2092,6 @@
     <mergeCell ref="B32:F32"/>
     <mergeCell ref="B33:F33"/>
     <mergeCell ref="A22:J22"/>
-    <mergeCell ref="B23:F23"/>
-    <mergeCell ref="B24:F24"/>
-    <mergeCell ref="B25:F25"/>
-    <mergeCell ref="B26:F26"/>
-    <mergeCell ref="B27:F27"/>
-    <mergeCell ref="B14:H14"/>
-    <mergeCell ref="A15:J15"/>
-    <mergeCell ref="A16:J16"/>
-    <mergeCell ref="A18:J18"/>
-    <mergeCell ref="A20:J20"/>
-    <mergeCell ref="A21:J21"/>
-    <mergeCell ref="B8:F8"/>
-    <mergeCell ref="B9:H9"/>
-    <mergeCell ref="B10:H10"/>
-    <mergeCell ref="B11:F11"/>
-    <mergeCell ref="B12:F12"/>
-    <mergeCell ref="B13:H13"/>
-    <mergeCell ref="B2:H2"/>
-    <mergeCell ref="B3:H3"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="B5:H5"/>
-    <mergeCell ref="B6:H6"/>
-    <mergeCell ref="B7:F7"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>

</xml_diff>